<commit_message>
Keep track of my scanning
</commit_message>
<xml_diff>
--- a/data/scanningRecords.xlsx
+++ b/data/scanningRecords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\PhD_thesis\mast_growth\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D7E57E-F748-4968-B41E-83A16A6C7D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC532021-A8F9-4845-9A6A-1D3DDC1909B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
   <si>
     <t>treeID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -164,6 +164,14 @@
   </si>
   <si>
     <t>5549(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -531,6 +539,9 @@
       <c r="D2">
         <v>60</v>
       </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
       <c r="F2" s="1">
         <v>45922</v>
       </c>
@@ -548,8 +559,11 @@
       <c r="D3">
         <v>60</v>
       </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
       <c r="F3" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -565,6 +579,9 @@
       <c r="D4">
         <v>60</v>
       </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
       <c r="F4" s="1">
         <v>45922</v>
       </c>
@@ -582,8 +599,11 @@
       <c r="D5">
         <v>60</v>
       </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
       <c r="F5" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -599,6 +619,9 @@
       <c r="D6">
         <v>60</v>
       </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="1">
         <v>45922</v>
       </c>
@@ -616,8 +639,11 @@
       <c r="D7">
         <v>60</v>
       </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
       <c r="F7" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -633,8 +659,11 @@
       <c r="D8">
         <v>60</v>
       </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -650,6 +679,9 @@
       <c r="D9">
         <v>60</v>
       </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
       <c r="F9" s="1">
         <v>45922</v>
       </c>
@@ -667,8 +699,11 @@
       <c r="D10">
         <v>60</v>
       </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
       <c r="F10" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -684,8 +719,11 @@
       <c r="D11">
         <v>60</v>
       </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
       <c r="F11" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -701,8 +739,11 @@
       <c r="D12">
         <v>60</v>
       </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
       <c r="F12" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -718,6 +759,9 @@
       <c r="D13">
         <v>60</v>
       </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
       <c r="F13" s="1">
         <v>45922</v>
       </c>
@@ -736,7 +780,7 @@
         <v>60</v>
       </c>
       <c r="F14" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -753,7 +797,7 @@
         <v>60</v>
       </c>
       <c r="F15" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -770,7 +814,7 @@
         <v>60</v>
       </c>
       <c r="F16" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -787,7 +831,7 @@
         <v>60</v>
       </c>
       <c r="F17" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -804,7 +848,7 @@
         <v>60</v>
       </c>
       <c r="F18" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -820,9 +864,7 @@
       <c r="D19">
         <v>60</v>
       </c>
-      <c r="F19" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -837,9 +879,7 @@
       <c r="D20">
         <v>60</v>
       </c>
-      <c r="F20" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -854,9 +894,7 @@
       <c r="D21">
         <v>60</v>
       </c>
-      <c r="F21" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -871,9 +909,7 @@
       <c r="D22">
         <v>60</v>
       </c>
-      <c r="F22" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -888,9 +924,7 @@
       <c r="D23">
         <v>60</v>
       </c>
-      <c r="F23" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -905,9 +939,7 @@
       <c r="D24">
         <v>60</v>
       </c>
-      <c r="F24" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -922,9 +954,7 @@
       <c r="D25">
         <v>60</v>
       </c>
-      <c r="F25" s="1">
-        <v>45922</v>
-      </c>
+      <c r="F25" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
keep track of scanning
</commit_message>
<xml_diff>
--- a/data/scanningRecords.xlsx
+++ b/data/scanningRecords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\PhD_thesis\mast_growth\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC532021-A8F9-4845-9A6A-1D3DDC1909B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5393E8D-A5D0-4357-972D-24E83935F578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>treeID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,6 +172,22 @@
   </si>
   <si>
     <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5502(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5502(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5543(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5543(2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -560,7 +576,7 @@
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>45924</v>
@@ -600,7 +616,7 @@
         <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1">
         <v>45924</v>
@@ -640,7 +656,7 @@
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1">
         <v>45924</v>
@@ -660,7 +676,7 @@
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1">
         <v>45924</v>
@@ -700,7 +716,7 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1">
         <v>45924</v>
@@ -720,7 +736,7 @@
         <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1">
         <v>45924</v>
@@ -740,7 +756,7 @@
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1">
         <v>45924</v>
@@ -779,6 +795,9 @@
       <c r="D14">
         <v>60</v>
       </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
       <c r="F14" s="1">
         <v>45924</v>
       </c>
@@ -796,6 +815,9 @@
       <c r="D15">
         <v>60</v>
       </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
       <c r="F15" s="1">
         <v>45924</v>
       </c>
@@ -813,6 +835,9 @@
       <c r="D16">
         <v>60</v>
       </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
       <c r="F16" s="1">
         <v>45924</v>
       </c>
@@ -830,6 +855,9 @@
       <c r="D17">
         <v>60</v>
       </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
       <c r="F17" s="1">
         <v>45924</v>
       </c>
@@ -847,8 +875,11 @@
       <c r="D18">
         <v>60</v>
       </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
       <c r="F18" s="1">
-        <v>45924</v>
+        <v>45925</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -864,7 +895,9 @@
       <c r="D19">
         <v>60</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1">
+        <v>45925</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -879,7 +912,9 @@
       <c r="D20">
         <v>60</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1">
+        <v>45925</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -894,7 +929,9 @@
       <c r="D21">
         <v>60</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1">
+        <v>45925</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -909,7 +946,9 @@
       <c r="D22">
         <v>60</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1">
+        <v>45925</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -924,7 +963,9 @@
       <c r="D23">
         <v>60</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1">
+        <v>45925</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -939,7 +980,9 @@
       <c r="D24">
         <v>60</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1">
+        <v>45925</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -954,7 +997,77 @@
       <c r="D25">
         <v>60</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1">
+        <v>45925</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>60</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45925</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>60</v>
+      </c>
+      <c r="F27" s="1">
+        <v>45925</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>60</v>
+      </c>
+      <c r="F28" s="1">
+        <v>45925</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>60</v>
+      </c>
+      <c r="F29" s="1">
+        <v>45925</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>